<commit_message>
multiple LEDs option added
</commit_message>
<xml_diff>
--- a/designs/Pufferfish-Interface-1/reference/Interface BOM Draft.xlsx
+++ b/designs/Pufferfish-Interface-1/reference/Interface BOM Draft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenadachi/Documents/GitHub/pufferfish-electronics/designs/Pufferfish-Interface-1/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CC0A07-D847-F541-86A3-2E52AAE9F466}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1ECDED-1A2D-C746-A946-6A2889B3B623}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="1880" windowWidth="21340" windowHeight="14540" xr2:uid="{C443EF20-858B-934F-A0C9-B37FE8547315}"/>
+    <workbookView xWindow="1880" yWindow="460" windowWidth="21340" windowHeight="14540" xr2:uid="{C443EF20-858B-934F-A0C9-B37FE8547315}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2562" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2566" uniqueCount="457">
   <si>
     <t>/export</t>
   </si>
@@ -1432,9 +1432,6 @@
     <t>B2B-PH-SM4-TB(LF)(SN)</t>
   </si>
   <si>
-    <t>find one</t>
-  </si>
-  <si>
     <t>Buzzer_PS1927P02</t>
   </si>
   <si>
@@ -1442,6 +1439,18 @@
   </si>
   <si>
     <t>Connector to Control Board</t>
+  </si>
+  <si>
+    <t>Keep in mind we need a protective guard cover thing</t>
+  </si>
+  <si>
+    <t>5103308-3</t>
+  </si>
+  <si>
+    <t>In library</t>
+  </si>
+  <si>
+    <t>IN library</t>
   </si>
 </sst>
 </file>
@@ -1606,7 +1615,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1653,6 +1662,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1971,7 +1981,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2033,7 +2043,7 @@
         <v>409</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>407</v>
@@ -2158,7 +2168,9 @@
       <c r="F9" s="17" t="s">
         <v>384</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="15" t="s">
+        <v>453</v>
+      </c>
       <c r="H9" s="15"/>
       <c r="I9" s="28"/>
       <c r="J9" s="16"/>
@@ -2194,7 +2206,7 @@
         <v>441</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D11" s="25" t="s">
         <v>442</v>
@@ -2214,9 +2226,11 @@
       <c r="B12" s="6" t="s">
         <v>445</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="19" t="s">
-        <v>450</v>
+      <c r="C12" s="21" t="s">
+        <v>456</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>456</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="6"/>
@@ -2316,11 +2330,15 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="21" t="s">
-        <v>453</v>
-      </c>
-      <c r="B17" s="4"/>
+        <v>452</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>454</v>
+      </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="34" t="s">
+        <v>455</v>
+      </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>

</xml_diff>

<commit_message>
TVS diode update (passes DFM)
</commit_message>
<xml_diff>
--- a/designs/Pufferfish-Interface-1/reference/Interface BOM Draft.xlsx
+++ b/designs/Pufferfish-Interface-1/reference/Interface BOM Draft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenadachi/Documents/GitHub/pufferfish-electronics/designs/Pufferfish-Interface-1/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEADACE-22BE-5948-9BFE-1F45C8D49487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FA8C64-A6F0-9B4E-897F-1AE9E35E62D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2320" windowWidth="25600" windowHeight="14520" xr2:uid="{C443EF20-858B-934F-A0C9-B37FE8547315}"/>
+    <workbookView xWindow="7080" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{C443EF20-858B-934F-A0C9-B37FE8547315}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2567" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2568" uniqueCount="457">
   <si>
     <t>/export</t>
   </si>
@@ -1184,9 +1184,6 @@
     <t>https://www.onsemi.com/pub/Collateral/KSC1815-D.pdf</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/TPD1E1B04DPYR?qs=LuYMPh7GGMTwEWL%2FIe5IJQ%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.vishay.com/docs/70860/70860.pdf</t>
   </si>
   <si>
@@ -1256,9 +1253,6 @@
     <t>0805 SMD RES</t>
   </si>
   <si>
-    <t xml:space="preserve">TPD1E1B04 </t>
-  </si>
-  <si>
     <t>Alarm 2 (reg) diodes</t>
   </si>
   <si>
@@ -1386,13 +1380,25 @@
   </si>
   <si>
     <t>See B2B, same but w/ 4 ports</t>
+  </si>
+  <si>
+    <t>https://www.littelfuse.com/~/media/electronics/datasheets/tvs_diodes/littelfuse_tvs_diode_smf3_3_datasheet.pdf.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/littelfuse-inc/SMF3-3/F7701TR-ND/6189040</t>
+  </si>
+  <si>
+    <t>SMF3.3</t>
+  </si>
+  <si>
+    <t>Specified in datasheet, SMD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1493,12 +1499,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1549,7 +1549,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1569,18 +1569,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1899,7 +1896,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1912,7 +1909,7 @@
     <row r="1" spans="1:12">
       <c r="A1" s="5"/>
       <c r="B1" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>380</v>
@@ -1925,70 +1922,70 @@
         <v>383</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>401</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>402</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>90</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>403</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>405</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>435</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>404</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H4" s="5"/>
     </row>
@@ -1997,7 +1994,7 @@
         <v>384</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>216</v>
@@ -2008,19 +2005,19 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>394</v>
-      </c>
       <c r="C6" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>101</v>
@@ -2034,10 +2031,10 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>386</v>
@@ -2047,52 +2044,52 @@
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>118</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>441</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>442</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>443</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>444</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="14" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H9" s="5"/>
       <c r="J9" s="13"/>
@@ -2103,52 +2100,52 @@
       <c r="A10" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>411</v>
+      <c r="B10" s="4" t="s">
+        <v>455</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="D10" s="17">
-        <v>402</v>
-      </c>
-      <c r="E10" s="17"/>
+        <v>453</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>456</v>
+      </c>
+      <c r="E10" s="16"/>
       <c r="F10" s="14" t="s">
-        <v>387</v>
+        <v>454</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
-        <v>439</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>440</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>454</v>
-      </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+        <v>437</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>438</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>452</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="14"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="B12" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>445</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="14" t="s">
         <v>447</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>448</v>
-      </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="14" t="s">
-        <v>449</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -2156,16 +2153,16 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>216</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -2174,93 +2171,93 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>449</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="5" t="s">
         <v>450</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>451</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="5" t="s">
-        <v>452</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="5" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B15" s="11">
         <v>190160099</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="5" t="s">
-        <v>416</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>433</v>
+        <v>414</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>431</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>434</v>
+        <v>413</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>432</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -2273,14 +2270,12 @@
     <hyperlink ref="C8" r:id="rId3" xr:uid="{D102AEE5-2D42-644E-A41C-09342F3628A3}"/>
     <hyperlink ref="C3" r:id="rId4" xr:uid="{26C66933-4B8E-F043-B399-E50B4F069CCF}"/>
     <hyperlink ref="C2" r:id="rId5" xr:uid="{4F9DE837-640F-C546-AF85-69233416E9D7}"/>
-    <hyperlink ref="C10" r:id="rId6" xr:uid="{D1C06134-AF0C-F148-A422-7919924EE480}"/>
-    <hyperlink ref="F10" r:id="rId7" xr:uid="{EB2C928C-9695-F149-96D9-F709CF9FC9C4}"/>
-    <hyperlink ref="F3" r:id="rId8" xr:uid="{36B935D2-D499-EF4F-8459-4DD0DA07D646}"/>
-    <hyperlink ref="F2" r:id="rId9" xr:uid="{74B06F71-75A5-564E-B6AE-421EC3BE759D}"/>
-    <hyperlink ref="F6" r:id="rId10" display="https://www.digikey.com/product-detail/en/vishay-siliconix/2N7002E-T1-E3/2N7002E-T1-E3CT-ND/3946142?utm_adgroup=Semiconductor%20Modules&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_RLSA_Buyers&amp;utm_term=&amp;utm_content=Semiconductor%20Modules&amp;gclid=Cj0KCQjwrIf3BRD1ARIsAMuugNtAYg0B4uzN6uG3FDVYlywiEKFAGbXRLO8hnfXG_d9twvCOg1_5j4waAs4CEALw_wcB" xr:uid="{6AD03F77-DE02-2544-8A4F-1D4EF609DF3F}"/>
-    <hyperlink ref="F8" r:id="rId11" xr:uid="{B40E1448-B7F4-A84B-B214-5C6DE8620A0F}"/>
-    <hyperlink ref="F7" r:id="rId12" xr:uid="{2EA15958-B5F2-344F-B464-AC3BF923BF86}"/>
-    <hyperlink ref="D17" r:id="rId13" xr:uid="{F6057F65-52ED-164F-A980-EDA142320DEB}"/>
+    <hyperlink ref="F3" r:id="rId6" xr:uid="{36B935D2-D499-EF4F-8459-4DD0DA07D646}"/>
+    <hyperlink ref="F2" r:id="rId7" xr:uid="{74B06F71-75A5-564E-B6AE-421EC3BE759D}"/>
+    <hyperlink ref="F6" r:id="rId8" display="https://www.digikey.com/product-detail/en/vishay-siliconix/2N7002E-T1-E3/2N7002E-T1-E3CT-ND/3946142?utm_adgroup=Semiconductor%20Modules&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_RLSA_Buyers&amp;utm_term=&amp;utm_content=Semiconductor%20Modules&amp;gclid=Cj0KCQjwrIf3BRD1ARIsAMuugNtAYg0B4uzN6uG3FDVYlywiEKFAGbXRLO8hnfXG_d9twvCOg1_5j4waAs4CEALw_wcB" xr:uid="{6AD03F77-DE02-2544-8A4F-1D4EF609DF3F}"/>
+    <hyperlink ref="F8" r:id="rId9" xr:uid="{B40E1448-B7F4-A84B-B214-5C6DE8620A0F}"/>
+    <hyperlink ref="F7" r:id="rId10" xr:uid="{2EA15958-B5F2-344F-B464-AC3BF923BF86}"/>
+    <hyperlink ref="D17" r:id="rId11" xr:uid="{F6057F65-52ED-164F-A980-EDA142320DEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>